<commit_message>
update ATRX mutation based on MAF, to include VUS
</commit_message>
<xml_diff>
--- a/analyses/07-additional_figures/output/hgat_tmb_mut_counts_df.xlsx
+++ b/analyses/07-additional_figures/output/hgat_tmb_mut_counts_df.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t xml:space="preserve">Tumor_Sample_Barcode</t>
   </si>
@@ -23,10 +23,16 @@
     <t xml:space="preserve">TMB Coding</t>
   </si>
   <si>
+    <t xml:space="preserve">sample_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">alt final</t>
   </si>
   <si>
-    <t xml:space="preserve">atrx_mut</t>
+    <t xml:space="preserve">ONCOGENIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atrx_mut_updated</t>
   </si>
   <si>
     <t xml:space="preserve">log2_mut_count</t>
@@ -35,268 +41,532 @@
     <t xml:space="preserve">BS_20TBZG09</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-515</t>
+  </si>
+  <si>
     <t xml:space="preserve">POS</t>
   </si>
   <si>
+    <t xml:space="preserve">Likely Oncogenic</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATRX_mut</t>
   </si>
   <si>
     <t xml:space="preserve">BS_CGXTFM67</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3212</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEG</t>
   </si>
   <si>
+    <t xml:space="preserve">Not mutated</t>
+  </si>
+  <si>
     <t xml:space="preserve">non_ATRX_mut</t>
   </si>
   <si>
     <t xml:space="preserve">BS_VW4XN9Y7</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2640</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_02YBZSBY</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2189</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_S0T3CQ97</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2980</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_TRGECFNP</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VUS</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_85Q5P8GF</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2594</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_P3PF53V8</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2307</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_3E5C1PN1</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1937</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_3BMGF6GN</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1656</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_R6CKWZW6</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3222</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_3NX3RBCX</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-114</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_CBMAWSAR</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3227</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_872Q3FK2</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-903</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_JB3J82ZK</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2308</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_M5FM63EB</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3214</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_WPCBK1EG</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1763</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_EPM623G4</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1099</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_BQ81D2BP</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3223</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_D6XHKZDZ</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-89</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_ABZ3BK38</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3000</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_MW63FCZC</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-535</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_H0638GZT</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-392</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_EJV0N3BX</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2217</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_1S5V7WWC</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3771</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_1M63B97V</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2751</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_9DM8H1RX</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-194</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_80078QDG</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3765</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_79NQJZ09</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1774</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_KAD49R68</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3521</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_928HWFFM</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2561</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_P8WN8XEQ</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1105</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_230S192D</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1956</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_YB99Q6TN</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2557</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_BFDEZK1C</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1102</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_C19DFVR5</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-343</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_742CDKAS</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-913</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_79SYEHY3</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3022</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_M4E4H6NG</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2288</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_KSHETTQC</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2176</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_8FSJDG2T</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3030</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_AFAHY6HP</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-46</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_Q6GVRAWK</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3225</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_TQ0J7WJQ</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3219</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_3Z40EZHD</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3213</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_FKQ7F6D1</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3122</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_SK4H5MJQ</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-204</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_YHXMYDBN</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3231</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_1MME7FBS</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3216</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_EP25TTAG</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2140</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_ZCY4ECNV</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1085</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_PPY0EWPG</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-116</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_P4K6WK9Y</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-461</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_KHSYAB3J</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2152</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_WJB33V17</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3769</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_W2QCHQ7E</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-161</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_7GKF6M85</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3224</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_B9QP40ER</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-409</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_FK3B5SDH</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3221</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_7PF3C1P7</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3218</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_G9MQM1KK</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-445</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_F064HMTP</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3625</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_S791VC80</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2737</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_KXGJ1HMG</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-870</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_F8K4VQMF</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3817</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_XGVSX8BX</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2610</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_RG6JK7ZN</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2100</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_R1G6SG0K</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-440</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_STNH7YSX</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-158</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_23ZE42Q3</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3206</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_KYPMZZSY</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-1708</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_T7WMJ08W</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-466</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_DH86PF5A</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3208</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_MSB1RDAJ</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-71</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_E42SSQGJ</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-85</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_SKRY0BJ4</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2151</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_NNFDFAFM</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3215</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_AYPBAHJ6</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-195</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_WJF6ZXWN</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-3935</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_823V5X6Z</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-388</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_1YTHM07J</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-325</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_GKPVZXYP</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-644</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_HJ95JNFN</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2274</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_QWS88QXE</t>
   </si>
   <si>
+    <t xml:space="preserve">7316-2857</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_NJFK43N3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7316-3075</t>
   </si>
 </sst>
 </file>
@@ -647,10 +917,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
         <v>8646</v>
@@ -659,18 +935,24 @@
         <v>307.049216710925</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="n">
         <v>13.0778171208959</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
         <v>15</v>
@@ -679,18 +961,24 @@
         <v>0.139987789145128</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="n">
         <v>3.90689059560852</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4" t="n">
         <v>5796</v>
@@ -699,18 +987,24 @@
         <v>187.387654549669</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="n">
         <v>12.5008418795569</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>7163</v>
@@ -719,18 +1013,24 @@
         <v>274.488056955768</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="n">
         <v>12.8063482267123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B6" t="n">
         <v>293</v>
@@ -739,18 +1039,24 @@
         <v>7.75532351864012</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="n">
         <v>8.19475685442225</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B7" t="n">
         <v>44</v>
@@ -759,18 +1065,24 @@
         <v>1.11990231316103</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="n">
         <v>5.4594316186373</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B8" t="n">
         <v>192</v>
@@ -779,18 +1091,24 @@
         <v>4.73158727310534</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="n">
         <v>7.58496250072116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B9" t="n">
         <v>573</v>
@@ -799,18 +1117,24 @@
         <v>15.4826494794512</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="n">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="n">
         <v>9.16239132875691</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B10" t="n">
         <v>22</v>
@@ -819,18 +1143,24 @@
         <v>0.531953598751488</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" t="n">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="n">
         <v>4.4594316186373</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B11" t="n">
         <v>60</v>
@@ -839,18 +1169,24 @@
         <v>1.00791208184492</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="n">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="n">
         <v>5.90689059560852</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B12" t="n">
         <v>20</v>
@@ -859,18 +1195,24 @@
         <v>0.475958483093437</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="n">
         <v>4.32192809488736</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B13" t="n">
         <v>37</v>
@@ -879,18 +1221,24 @@
         <v>0.923919408357848</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="n">
         <v>5.20945336562895</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B14" t="n">
         <v>22</v>
@@ -899,18 +1247,24 @@
         <v>0.503956040922462</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="n">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="n">
         <v>4.4594316186373</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B15" t="n">
         <v>91</v>
@@ -919,18 +1273,24 @@
         <v>2.21180706849303</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" t="n">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="n">
         <v>6.5077946401987</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B16" t="n">
         <v>74</v>
@@ -939,18 +1299,24 @@
         <v>1.65185591191252</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="n">
         <v>6.20945336562895</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B17" t="n">
         <v>25</v>
@@ -959,18 +1325,24 @@
         <v>0.587948714409539</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="n">
         <v>4.64385618977472</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B18" t="n">
         <v>28</v>
@@ -979,18 +1351,24 @@
         <v>0.643943830067591</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="n">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="n">
         <v>4.8073549220576</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B19" t="n">
         <v>49</v>
@@ -999,18 +1377,24 @@
         <v>1.14789987099005</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" t="n">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="n">
         <v>5.61470984411521</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B20" t="n">
         <v>11</v>
@@ -1019,18 +1403,24 @@
         <v>0.223980462632206</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="n">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="n">
         <v>3.4594316186373</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B21" t="n">
         <v>4</v>
@@ -1039,18 +1429,24 @@
         <v>0.0839926734870771</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="n">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B22" t="n">
         <v>36</v>
@@ -1059,18 +1455,24 @@
         <v>0.727936503554668</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="n">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="n">
         <v>5.16992500144231</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B23" t="n">
         <v>15</v>
@@ -1079,18 +1481,24 @@
         <v>0.279975578290257</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="n">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="n">
         <v>3.90689059560852</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B24" t="n">
         <v>27</v>
@@ -1099,18 +1507,24 @@
         <v>0.615946272238565</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="n">
         <v>4.75488750216347</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B25" t="n">
         <v>38</v>
@@ -1119,18 +1533,24 @@
         <v>0.895921850528822</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="n">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="n">
         <v>5.24792751344359</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B26" t="n">
         <v>27</v>
@@ -1139,18 +1559,24 @@
         <v>0.615946272238565</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" t="n">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="n">
         <v>4.75488750216347</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B27" t="n">
         <v>66</v>
@@ -1159,18 +1585,24 @@
         <v>1.79184370105764</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" t="n">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="n">
         <v>6.04439411935845</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B28" t="n">
         <v>8</v>
@@ -1179,18 +1611,24 @@
         <v>0.167985346974154</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" t="n">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B29" t="n">
         <v>64</v>
@@ -1199,18 +1637,24 @@
         <v>1.53986568059641</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" t="n">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B30" t="n">
         <v>28</v>
@@ -1219,18 +1663,24 @@
         <v>0.671941387896617</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" t="n">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" t="n">
         <v>4.8073549220576</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B31" t="n">
         <v>30</v>
@@ -1239,18 +1689,24 @@
         <v>0.727936503554668</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="n">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="n">
         <v>4.90689059560852</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B32" t="n">
         <v>188</v>
@@ -1259,18 +1715,24 @@
         <v>1.76384614322862</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" t="n">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="n">
         <v>7.55458885167764</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B33" t="n">
         <v>158</v>
@@ -1279,18 +1741,24 @@
         <v>3.61168495994431</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" t="n">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="n">
         <v>7.3037807481771</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="B34" t="n">
         <v>35</v>
@@ -1299,18 +1767,24 @@
         <v>0.839926734870771</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" t="n">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="n">
         <v>5.12928301694497</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B35" t="n">
         <v>14</v>
@@ -1319,18 +1793,24 @@
         <v>0.363968251777334</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="n">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" t="n">
         <v>3.8073549220576</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="B36" t="n">
         <v>26</v>
@@ -1339,18 +1819,24 @@
         <v>0.643943830067591</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" t="n">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="n">
         <v>4.70043971814109</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B37" t="n">
         <v>20</v>
@@ -1359,18 +1845,24 @@
         <v>0.503956040922462</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" t="n">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="n">
         <v>4.32192809488736</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="B38" t="n">
         <v>76</v>
@@ -1379,18 +1871,24 @@
         <v>1.9598290480318</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" t="n">
+        <v>15</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" t="n">
         <v>6.24792751344359</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B39" t="n">
         <v>94</v>
@@ -1399,18 +1897,24 @@
         <v>2.49178264678329</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" t="n">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" t="n">
         <v>6.55458885167764</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="B40" t="n">
         <v>41</v>
@@ -1419,18 +1923,24 @@
         <v>1.00791208184492</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" t="n">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" t="n">
         <v>5.35755200461808</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="B41" t="n">
         <v>2</v>
@@ -1439,18 +1949,24 @@
         <v>0.0279975578290257</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" t="n">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="B42" t="n">
         <v>28</v>
@@ -1459,18 +1975,24 @@
         <v>0.587948714409539</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" t="n">
+        <v>15</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" t="n">
         <v>4.8073549220576</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B43" t="n">
         <v>26</v>
@@ -1479,18 +2001,24 @@
         <v>0.419963367435385</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" t="n">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" t="n">
         <v>4.70043971814109</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="B44" t="n">
         <v>8</v>
@@ -1499,18 +2027,24 @@
         <v>0.167985346974154</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" t="n">
+        <v>15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="B45" t="n">
         <v>19</v>
@@ -1519,18 +2053,24 @@
         <v>0.39196580960636</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" t="n">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="n">
         <v>4.24792751344359</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="B46" t="n">
         <v>18</v>
@@ -1539,18 +2079,24 @@
         <v>0.307973136119283</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" t="n">
+        <v>15</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" t="n">
         <v>4.16992500144231</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B47" t="n">
         <v>34</v>
@@ -1559,18 +2105,24 @@
         <v>0.811929177041745</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
-      </c>
-      <c r="F47" t="n">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="n">
         <v>5.08746284125034</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="B48" t="n">
         <v>32</v>
@@ -1579,18 +2131,24 @@
         <v>0.895921850528822</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" t="n">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B49" t="n">
         <v>42</v>
@@ -1599,18 +2157,24 @@
         <v>1.06390719750298</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" t="n">
+        <v>15</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="n">
         <v>5.39231742277876</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="B50" t="n">
         <v>24</v>
@@ -1619,18 +2183,24 @@
         <v>0.615946272238565</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" t="n">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="n">
         <v>4.58496250072116</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B51" t="n">
         <v>43</v>
@@ -1639,18 +2209,24 @@
         <v>1.00791208184492</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" t="n">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="n">
         <v>5.4262647547021</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B52" t="n">
         <v>26</v>
@@ -1659,18 +2235,24 @@
         <v>0.503956040922462</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>116</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" t="n">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" t="n">
         <v>4.70043971814109</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="B53" t="n">
         <v>36</v>
@@ -1679,18 +2261,24 @@
         <v>0.615946272238565</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" t="n">
+        <v>15</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" t="n">
         <v>5.16992500144231</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="B54" t="n">
         <v>72</v>
@@ -1699,18 +2287,24 @@
         <v>1.70785102757057</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" t="n">
+        <v>15</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H54" t="n">
         <v>6.16992500144231</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="B55" t="n">
         <v>46</v>
@@ -1719,18 +2313,24 @@
         <v>1.23189254447713</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" t="n">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" t="n">
         <v>5.52356195605701</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="B56" t="n">
         <v>12</v>
@@ -1739,18 +2339,24 @@
         <v>0.279975578290257</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" t="n">
+        <v>15</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+      <c r="G56" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" t="n">
         <v>3.58496250072116</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="B57" t="n">
         <v>31</v>
@@ -1759,18 +2365,24 @@
         <v>0.643943830067591</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" t="n">
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" t="n">
         <v>4.95419631038687</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="B58" t="n">
         <v>25</v>
@@ -1779,18 +2391,24 @@
         <v>0.503956040922462</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" t="n">
+        <v>15</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" t="n">
         <v>4.64385618977472</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="B59" t="n">
         <v>14</v>
@@ -1799,18 +2417,24 @@
         <v>0.223980462632206</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
-      </c>
-      <c r="F59" t="n">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="n">
         <v>3.8073549220576</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
       <c r="B60" t="n">
         <v>8</v>
@@ -1819,18 +2443,24 @@
         <v>0.111990231316103</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" t="n">
+        <v>15</v>
+      </c>
+      <c r="F60" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="B61" t="n">
         <v>16</v>
@@ -1839,18 +2469,24 @@
         <v>0.19598290480318</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" t="n">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="B62" t="n">
         <v>26</v>
@@ -1859,18 +2495,24 @@
         <v>0.643943830067591</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
-      </c>
-      <c r="F62" t="n">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" t="n">
         <v>4.70043971814109</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="B63" t="n">
         <v>6</v>
@@ -1879,18 +2521,24 @@
         <v>0.0559951156580514</v>
       </c>
       <c r="D63" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" t="n">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
+        <v>17</v>
+      </c>
+      <c r="H63" t="n">
         <v>2.58496250072116</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="B64" t="n">
         <v>90</v>
@@ -1899,18 +2547,24 @@
         <v>2.12781439500595</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" t="n">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" t="n">
         <v>6.49185309632967</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B65" t="n">
         <v>16</v>
@@ -1919,18 +2573,24 @@
         <v>0.419963367435385</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>142</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" t="n">
+        <v>15</v>
+      </c>
+      <c r="F65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="B66" t="n">
         <v>29</v>
@@ -1939,18 +2599,24 @@
         <v>0.699938945725642</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" t="n">
+        <v>15</v>
+      </c>
+      <c r="F66" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66" t="n">
         <v>4.85798099512757</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="B67" t="n">
         <v>26</v>
@@ -1959,18 +2625,24 @@
         <v>0.615946272238565</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" t="n">
+        <v>15</v>
+      </c>
+      <c r="F67" t="s">
+        <v>26</v>
+      </c>
+      <c r="G67" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" t="n">
         <v>4.70043971814109</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="B68" t="n">
         <v>15</v>
@@ -1979,18 +2651,24 @@
         <v>0.363968251777334</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>148</v>
       </c>
       <c r="E68" t="s">
-        <v>8</v>
-      </c>
-      <c r="F68" t="n">
+        <v>10</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" t="n">
         <v>3.90689059560852</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="B69" t="n">
         <v>28</v>
@@ -1999,18 +2677,24 @@
         <v>0.615946272238565</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" t="n">
+        <v>15</v>
+      </c>
+      <c r="F69" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" t="n">
         <v>4.8073549220576</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="B70" t="n">
         <v>30</v>
@@ -2019,18 +2703,24 @@
         <v>0.671941387896617</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="E70" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" t="n">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70" t="n">
         <v>4.90689059560852</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="B71" t="n">
         <v>29</v>
@@ -2039,18 +2729,24 @@
         <v>0.727936503554668</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>154</v>
       </c>
       <c r="E71" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" t="n">
+        <v>10</v>
+      </c>
+      <c r="F71" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" t="n">
         <v>4.85798099512757</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="B72" t="n">
         <v>36</v>
@@ -2059,18 +2755,24 @@
         <v>0.671941387896617</v>
       </c>
       <c r="D72" t="s">
-        <v>7</v>
+        <v>156</v>
       </c>
       <c r="E72" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" t="n">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" t="n">
         <v>5.16992500144231</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="B73" t="n">
         <v>14</v>
@@ -2079,18 +2781,24 @@
         <v>0.307973136119283</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>158</v>
       </c>
       <c r="E73" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" t="n">
+        <v>15</v>
+      </c>
+      <c r="F73" t="s">
+        <v>16</v>
+      </c>
+      <c r="G73" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" t="n">
         <v>3.8073549220576</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>159</v>
       </c>
       <c r="B74" t="n">
         <v>27</v>
@@ -2099,18 +2807,24 @@
         <v>0.587948714409539</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
-      </c>
-      <c r="F74" t="n">
+        <v>15</v>
+      </c>
+      <c r="F74" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74" t="n">
         <v>4.75488750216347</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
       <c r="B75" t="n">
         <v>16</v>
@@ -2119,18 +2833,24 @@
         <v>0.363968251777334</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="E75" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" t="n">
+        <v>15</v>
+      </c>
+      <c r="F75" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="B76" t="n">
         <v>6</v>
@@ -2139,18 +2859,24 @@
         <v>0.0839926734870771</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="E76" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" t="n">
+        <v>15</v>
+      </c>
+      <c r="F76" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" t="n">
         <v>2.58496250072116</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="B77" t="n">
         <v>18</v>
@@ -2159,18 +2885,24 @@
         <v>0.0839926734870771</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>166</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
-      </c>
-      <c r="F77" t="n">
+        <v>15</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" t="n">
         <v>4.16992500144231</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="B78" t="n">
         <v>20</v>
@@ -2179,18 +2911,24 @@
         <v>0.39196580960636</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" t="n">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" t="n">
         <v>4.32192809488736</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="B79" t="n">
         <v>30</v>
@@ -2199,18 +2937,24 @@
         <v>0.531953598751488</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>170</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" t="n">
+        <v>15</v>
+      </c>
+      <c r="F79" t="s">
+        <v>26</v>
+      </c>
+      <c r="G79" t="s">
+        <v>12</v>
+      </c>
+      <c r="H79" t="n">
         <v>4.90689059560852</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="B80" t="n">
         <v>14</v>
@@ -2219,18 +2963,24 @@
         <v>0.279975578290257</v>
       </c>
       <c r="D80" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" t="n">
+        <v>15</v>
+      </c>
+      <c r="F80" t="s">
+        <v>26</v>
+      </c>
+      <c r="G80" t="s">
+        <v>12</v>
+      </c>
+      <c r="H80" t="n">
         <v>3.8073549220576</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
       <c r="B81" t="n">
         <v>12</v>
@@ -2239,18 +2989,24 @@
         <v>0.251978020461231</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" t="n">
+        <v>15</v>
+      </c>
+      <c r="F81" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" t="s">
+        <v>17</v>
+      </c>
+      <c r="H81" t="n">
         <v>3.58496250072116</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="B82" t="n">
         <v>7</v>
@@ -2259,18 +3015,24 @@
         <v>0.0279975578290257</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>176</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" t="n">
+        <v>15</v>
+      </c>
+      <c r="F82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" t="n">
         <v>2.8073549220576</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="B83" t="n">
         <v>20</v>
@@ -2279,18 +3041,24 @@
         <v>0.363968251777334</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>178</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" t="n">
+        <v>15</v>
+      </c>
+      <c r="F83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" t="n">
         <v>4.32192809488736</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>179</v>
       </c>
       <c r="B84" t="n">
         <v>6</v>
@@ -2299,18 +3067,24 @@
         <v>0.0839926734870771</v>
       </c>
       <c r="D84" t="s">
-        <v>7</v>
+        <v>180</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" t="n">
+        <v>10</v>
+      </c>
+      <c r="F84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" t="n">
         <v>2.58496250072116</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>181</v>
       </c>
       <c r="B85" t="n">
         <v>3</v>
@@ -2319,18 +3093,24 @@
         <v>0.0279975578290257</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>182</v>
       </c>
       <c r="E85" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" t="n">
+        <v>15</v>
+      </c>
+      <c r="F85" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" t="s">
+        <v>17</v>
+      </c>
+      <c r="H85" t="n">
         <v>1.58496250072116</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="B86" t="n">
         <v>3</v>
@@ -2339,12 +3119,18 @@
         <v>0.0279975578290257</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>184</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" t="n">
+        <v>15</v>
+      </c>
+      <c r="F86" t="s">
+        <v>26</v>
+      </c>
+      <c r="G86" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" t="n">
         <v>1.58496250072116</v>
       </c>
     </row>

</xml_diff>